<commit_message>
Modificato il Javadoc, corretti i diagrammi e le tabelle Excel.
</commit_message>
<xml_diff>
--- a/Babysitter/Piano di test.xlsx
+++ b/Babysitter/Piano di test.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Pc\Desktop\Babysitter_Progetto\Babysitter\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9C7B1EED-FFCC-42B2-8A75-D2BC5D33B3D3}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{09909DA0-410B-43F6-884F-09F8CE1A8852}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3080" yWindow="3040" windowWidth="28800" windowHeight="15460" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="38620" windowHeight="21220" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Foglio1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="167" uniqueCount="139">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="166" uniqueCount="138">
   <si>
     <t>N</t>
   </si>
@@ -319,9 +319,6 @@
   </si>
   <si>
     <t>testEliminaIntervento()</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Istanzio gli attributi: </t>
   </si>
   <si>
     <t xml:space="preserve">        a.eliminaIntervento(1);
@@ -771,8 +768,6 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -791,6 +786,8 @@
     <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normale" xfId="0" builtinId="0"/>
@@ -1085,10 +1082,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A2:G74"/>
+  <dimension ref="B2:G74"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A58" workbookViewId="0">
-      <selection activeCell="D76" sqref="D76"/>
+      <selection activeCell="I67" sqref="I67"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1101,10 +1098,10 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:7" x14ac:dyDescent="0.35">
-      <c r="F2" s="4" t="s">
+      <c r="F2" s="10" t="s">
         <v>6</v>
       </c>
-      <c r="G2" s="5"/>
+      <c r="G2" s="11"/>
     </row>
     <row r="3" spans="2:7" ht="15" thickBot="1" x14ac:dyDescent="0.4"/>
     <row r="4" spans="2:7" ht="15" thickBot="1" x14ac:dyDescent="0.4">
@@ -1131,1053 +1128,1075 @@
       <c r="B5" s="3">
         <v>1</v>
       </c>
-      <c r="C5" s="9" t="s">
+      <c r="C5" s="7" t="s">
         <v>11</v>
       </c>
-      <c r="D5" s="10"/>
-      <c r="E5" s="10"/>
-      <c r="F5" s="10"/>
-      <c r="G5" s="11"/>
-    </row>
-    <row r="6" spans="2:7" ht="290.5" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="D5" s="8"/>
+      <c r="E5" s="8"/>
+      <c r="F5" s="8"/>
+      <c r="G5" s="9"/>
+    </row>
+    <row r="6" spans="2:7" ht="276" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B6" s="3">
         <v>2</v>
       </c>
-      <c r="C6" s="6" t="s">
+      <c r="C6" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="D6" s="8" t="s">
+      <c r="D6" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="E6" s="7" t="s">
+      <c r="E6" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="F6" s="7" t="s">
+      <c r="F6" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="G6" s="6"/>
+      <c r="G6" s="4"/>
     </row>
     <row r="7" spans="2:7" ht="38" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B7" s="3">
         <v>3</v>
       </c>
-      <c r="C7" s="9" t="s">
+      <c r="C7" s="7" t="s">
         <v>12</v>
       </c>
-      <c r="D7" s="10"/>
-      <c r="E7" s="10"/>
-      <c r="F7" s="10"/>
-      <c r="G7" s="11"/>
+      <c r="D7" s="8"/>
+      <c r="E7" s="8"/>
+      <c r="F7" s="8"/>
+      <c r="G7" s="9"/>
     </row>
     <row r="8" spans="2:7" ht="29.5" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B8" s="3">
         <v>4</v>
       </c>
-      <c r="C8" s="6" t="s">
+      <c r="C8" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="D8" s="7"/>
-      <c r="E8" s="7" t="s">
+      <c r="D8" s="5"/>
+      <c r="E8" s="5" t="s">
         <v>32</v>
       </c>
-      <c r="F8" s="7">
+      <c r="F8" s="5">
         <v>1000</v>
       </c>
-      <c r="G8" s="6"/>
+      <c r="G8" s="4"/>
     </row>
     <row r="9" spans="2:7" ht="38" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B9" s="3">
         <v>5</v>
       </c>
-      <c r="C9" s="9" t="s">
+      <c r="C9" s="7" t="s">
         <v>13</v>
       </c>
-      <c r="D9" s="10"/>
-      <c r="E9" s="10"/>
-      <c r="F9" s="10"/>
-      <c r="G9" s="11"/>
+      <c r="D9" s="8"/>
+      <c r="E9" s="8"/>
+      <c r="F9" s="8"/>
+      <c r="G9" s="9"/>
     </row>
     <row r="10" spans="2:7" ht="29.5" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B10" s="3">
         <v>6</v>
       </c>
-      <c r="C10" s="6" t="s">
+      <c r="C10" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="D10" s="7"/>
-      <c r="E10" s="7" t="s">
+      <c r="D10" s="5"/>
+      <c r="E10" s="5" t="s">
         <v>33</v>
       </c>
-      <c r="F10" s="7">
+      <c r="F10" s="5">
         <v>0</v>
       </c>
-      <c r="G10" s="6"/>
+      <c r="G10" s="4"/>
     </row>
     <row r="11" spans="2:7" ht="44" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B11" s="3">
         <v>7</v>
       </c>
-      <c r="C11" s="6" t="s">
+      <c r="C11" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="D11" s="7"/>
-      <c r="E11" s="7" t="s">
+      <c r="D11" s="5"/>
+      <c r="E11" s="5" t="s">
         <v>34</v>
       </c>
-      <c r="F11" s="7">
+      <c r="F11" s="5">
         <v>1</v>
       </c>
-      <c r="G11" s="6"/>
+      <c r="G11" s="4"/>
     </row>
     <row r="12" spans="2:7" ht="42" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B12" s="3">
         <v>8</v>
       </c>
-      <c r="C12" s="9" t="s">
+      <c r="C12" s="7" t="s">
         <v>17</v>
       </c>
-      <c r="D12" s="10"/>
-      <c r="E12" s="10"/>
-      <c r="F12" s="10"/>
-      <c r="G12" s="11"/>
+      <c r="D12" s="8"/>
+      <c r="E12" s="8"/>
+      <c r="F12" s="8"/>
+      <c r="G12" s="9"/>
     </row>
     <row r="13" spans="2:7" ht="44" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B13" s="3">
         <v>9</v>
       </c>
-      <c r="C13" s="6" t="s">
+      <c r="C13" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="D13" s="7" t="s">
+      <c r="D13" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="E13" s="7" t="s">
+      <c r="E13" s="5" t="s">
         <v>35</v>
       </c>
-      <c r="F13" s="7" t="s">
+      <c r="F13" s="5" t="s">
         <v>31</v>
       </c>
-      <c r="G13" s="6"/>
+      <c r="G13" s="4"/>
     </row>
     <row r="14" spans="2:7" ht="44" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B14" s="3">
         <v>10</v>
       </c>
-      <c r="C14" s="6" t="s">
+      <c r="C14" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="D14" s="7"/>
-      <c r="E14" s="7" t="s">
+      <c r="D14" s="5"/>
+      <c r="E14" s="5" t="s">
         <v>36</v>
       </c>
-      <c r="F14" s="7" t="s">
+      <c r="F14" s="5" t="s">
         <v>21</v>
       </c>
-      <c r="G14" s="6"/>
+      <c r="G14" s="4"/>
     </row>
     <row r="15" spans="2:7" ht="42.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B15" s="3">
         <v>11</v>
       </c>
-      <c r="C15" s="9" t="s">
+      <c r="C15" s="7" t="s">
         <v>22</v>
       </c>
-      <c r="D15" s="10"/>
-      <c r="E15" s="10"/>
-      <c r="F15" s="10"/>
-      <c r="G15" s="11"/>
+      <c r="D15" s="8"/>
+      <c r="E15" s="8"/>
+      <c r="F15" s="8"/>
+      <c r="G15" s="9"/>
     </row>
     <row r="16" spans="2:7" ht="44" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B16" s="3">
         <v>12</v>
       </c>
-      <c r="C16" s="6" t="s">
+      <c r="C16" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="D16" s="6" t="s">
+      <c r="D16" s="4" t="s">
         <v>24</v>
       </c>
-      <c r="E16" s="6" t="s">
+      <c r="E16" s="4" t="s">
         <v>37</v>
       </c>
-      <c r="F16" s="6" t="s">
+      <c r="F16" s="4" t="s">
         <v>25</v>
       </c>
-      <c r="G16" s="6"/>
+      <c r="G16" s="4"/>
     </row>
     <row r="17" spans="2:7" ht="44" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B17" s="3">
         <v>13</v>
       </c>
-      <c r="C17" s="9" t="s">
+      <c r="C17" s="7" t="s">
         <v>26</v>
       </c>
-      <c r="D17" s="10"/>
-      <c r="E17" s="10"/>
-      <c r="F17" s="10"/>
-      <c r="G17" s="11"/>
+      <c r="D17" s="8"/>
+      <c r="E17" s="8"/>
+      <c r="F17" s="8"/>
+      <c r="G17" s="9"/>
     </row>
     <row r="18" spans="2:7" ht="87.5" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B18" s="3">
         <v>14</v>
       </c>
-      <c r="C18" s="6" t="s">
+      <c r="C18" s="4" t="s">
         <v>27</v>
       </c>
-      <c r="D18" s="6" t="s">
+      <c r="D18" s="4" t="s">
         <v>24</v>
       </c>
-      <c r="E18" s="6" t="s">
+      <c r="E18" s="4" t="s">
         <v>38</v>
       </c>
-      <c r="F18" s="6" t="s">
+      <c r="F18" s="4" t="s">
         <v>28</v>
       </c>
-      <c r="G18" s="6"/>
+      <c r="G18" s="4"/>
     </row>
     <row r="19" spans="2:7" ht="46" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B19" s="3">
         <v>15</v>
       </c>
-      <c r="C19" s="9" t="s">
+      <c r="C19" s="7" t="s">
         <v>29</v>
       </c>
-      <c r="D19" s="10"/>
-      <c r="E19" s="10"/>
-      <c r="F19" s="10"/>
-      <c r="G19" s="11"/>
+      <c r="D19" s="8"/>
+      <c r="E19" s="8"/>
+      <c r="F19" s="8"/>
+      <c r="G19" s="9"/>
     </row>
     <row r="20" spans="2:7" ht="29.5" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B20" s="3">
         <v>16</v>
       </c>
-      <c r="C20" s="6" t="s">
+      <c r="C20" s="4" t="s">
         <v>30</v>
       </c>
-      <c r="D20" s="6" t="s">
+      <c r="D20" s="4" t="s">
         <v>51</v>
       </c>
-      <c r="E20" s="6" t="s">
+      <c r="E20" s="4" t="s">
         <v>39</v>
       </c>
-      <c r="F20" s="6">
+      <c r="F20" s="4">
         <v>1</v>
       </c>
-      <c r="G20" s="6"/>
+      <c r="G20" s="4"/>
     </row>
     <row r="21" spans="2:7" ht="44" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B21" s="3">
         <v>17</v>
       </c>
-      <c r="C21" s="6" t="s">
+      <c r="C21" s="4" t="s">
         <v>40</v>
       </c>
-      <c r="D21" s="6"/>
-      <c r="E21" s="6" t="s">
+      <c r="D21" s="4"/>
+      <c r="E21" s="4" t="s">
         <v>41</v>
       </c>
-      <c r="F21" s="6">
+      <c r="F21" s="4">
         <v>1</v>
       </c>
-      <c r="G21" s="6"/>
+      <c r="G21" s="4"/>
     </row>
     <row r="22" spans="2:7" ht="44" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B22" s="3">
         <v>18</v>
       </c>
-      <c r="C22" s="6" t="s">
+      <c r="C22" s="4" t="s">
         <v>42</v>
       </c>
-      <c r="D22" s="6"/>
-      <c r="E22" s="6" t="s">
+      <c r="D22" s="4"/>
+      <c r="E22" s="4" t="s">
         <v>43</v>
       </c>
-      <c r="F22" s="6">
+      <c r="F22" s="4">
         <v>2</v>
       </c>
-      <c r="G22" s="6"/>
+      <c r="G22" s="4"/>
     </row>
     <row r="23" spans="2:7" ht="36.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B23" s="3">
         <v>19</v>
       </c>
-      <c r="C23" s="9" t="s">
+      <c r="C23" s="7" t="s">
         <v>44</v>
       </c>
-      <c r="D23" s="10"/>
-      <c r="E23" s="10"/>
-      <c r="F23" s="10"/>
-      <c r="G23" s="11"/>
+      <c r="D23" s="8"/>
+      <c r="E23" s="8"/>
+      <c r="F23" s="8"/>
+      <c r="G23" s="9"/>
     </row>
     <row r="24" spans="2:7" ht="44" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B24" s="3">
         <v>20</v>
       </c>
-      <c r="C24" s="6" t="s">
+      <c r="C24" s="4" t="s">
         <v>45</v>
       </c>
-      <c r="D24" s="6" t="s">
+      <c r="D24" s="4" t="s">
         <v>50</v>
       </c>
-      <c r="E24" s="6" t="s">
+      <c r="E24" s="4" t="s">
         <v>46</v>
       </c>
-      <c r="F24" s="6">
+      <c r="F24" s="4">
         <v>2</v>
       </c>
-      <c r="G24" s="6"/>
+      <c r="G24" s="4"/>
     </row>
     <row r="25" spans="2:7" ht="39" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B25" s="3">
         <v>21</v>
       </c>
-      <c r="C25" s="9" t="s">
+      <c r="C25" s="7" t="s">
         <v>47</v>
       </c>
-      <c r="D25" s="10"/>
-      <c r="E25" s="10"/>
-      <c r="F25" s="10"/>
-      <c r="G25" s="11"/>
+      <c r="D25" s="8"/>
+      <c r="E25" s="8"/>
+      <c r="F25" s="8"/>
+      <c r="G25" s="9"/>
     </row>
     <row r="26" spans="2:7" ht="58.5" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B26" s="3">
         <v>22</v>
       </c>
-      <c r="C26" s="6" t="s">
+      <c r="C26" s="4" t="s">
         <v>48</v>
       </c>
-      <c r="D26" s="6" t="s">
+      <c r="D26" s="4" t="s">
         <v>49</v>
       </c>
-      <c r="E26" s="6" t="s">
+      <c r="E26" s="4" t="s">
         <v>52</v>
       </c>
-      <c r="F26" s="6" t="s">
+      <c r="F26" s="4" t="s">
         <v>53</v>
       </c>
-      <c r="G26" s="6"/>
+      <c r="G26" s="4"/>
     </row>
     <row r="27" spans="2:7" ht="42" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B27" s="3">
         <v>23</v>
       </c>
-      <c r="C27" s="9" t="s">
+      <c r="C27" s="7" t="s">
         <v>54</v>
       </c>
-      <c r="D27" s="10"/>
-      <c r="E27" s="10"/>
-      <c r="F27" s="10"/>
-      <c r="G27" s="11"/>
+      <c r="D27" s="8"/>
+      <c r="E27" s="8"/>
+      <c r="F27" s="8"/>
+      <c r="G27" s="9"/>
     </row>
     <row r="28" spans="2:7" ht="44" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B28" s="3">
         <v>24</v>
       </c>
-      <c r="C28" s="6" t="s">
-        <v>60</v>
-      </c>
-      <c r="D28" s="6" t="s">
+      <c r="C28" s="4" t="s">
+        <v>59</v>
+      </c>
+      <c r="D28" s="4" t="s">
         <v>49</v>
       </c>
-      <c r="E28" s="6" t="s">
-        <v>56</v>
-      </c>
-      <c r="F28" s="6">
+      <c r="E28" s="4" t="s">
+        <v>55</v>
+      </c>
+      <c r="F28" s="4">
         <v>1</v>
       </c>
-      <c r="G28" s="6"/>
+      <c r="G28" s="4"/>
     </row>
     <row r="29" spans="2:7" ht="44" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B29" s="3">
         <v>25</v>
       </c>
-      <c r="C29" s="6" t="s">
-        <v>61</v>
-      </c>
-      <c r="D29" s="6"/>
-      <c r="E29" s="6" t="s">
-        <v>57</v>
-      </c>
-      <c r="F29" s="6">
+      <c r="C29" s="4" t="s">
+        <v>60</v>
+      </c>
+      <c r="D29" s="4"/>
+      <c r="E29" s="4" t="s">
+        <v>56</v>
+      </c>
+      <c r="F29" s="4">
         <v>0</v>
       </c>
-      <c r="G29" s="6"/>
+      <c r="G29" s="4"/>
     </row>
     <row r="30" spans="2:7" ht="33" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B30" s="3">
         <v>26</v>
       </c>
-      <c r="C30" s="9" t="s">
-        <v>58</v>
-      </c>
-      <c r="D30" s="10"/>
-      <c r="E30" s="10"/>
-      <c r="F30" s="10"/>
-      <c r="G30" s="11"/>
+      <c r="C30" s="7" t="s">
+        <v>57</v>
+      </c>
+      <c r="D30" s="8"/>
+      <c r="E30" s="8"/>
+      <c r="F30" s="8"/>
+      <c r="G30" s="9"/>
     </row>
     <row r="31" spans="2:7" ht="44" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B31" s="3">
         <v>27</v>
       </c>
-      <c r="C31" s="6" t="s">
-        <v>59</v>
-      </c>
-      <c r="D31" s="6" t="s">
+      <c r="C31" s="4" t="s">
+        <v>58</v>
+      </c>
+      <c r="D31" s="4" t="s">
+        <v>61</v>
+      </c>
+      <c r="E31" s="4" t="s">
         <v>62</v>
       </c>
-      <c r="E31" s="6" t="s">
-        <v>63</v>
-      </c>
-      <c r="F31" s="6">
+      <c r="F31" s="4">
         <v>1</v>
       </c>
-      <c r="G31" s="6"/>
+      <c r="G31" s="4"/>
     </row>
     <row r="32" spans="2:7" ht="33" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B32" s="3">
         <v>28</v>
       </c>
-      <c r="C32" s="9" t="s">
-        <v>64</v>
-      </c>
-      <c r="D32" s="10"/>
-      <c r="E32" s="10"/>
-      <c r="F32" s="10"/>
-      <c r="G32" s="11"/>
+      <c r="C32" s="7" t="s">
+        <v>63</v>
+      </c>
+      <c r="D32" s="8"/>
+      <c r="E32" s="8"/>
+      <c r="F32" s="8"/>
+      <c r="G32" s="9"/>
     </row>
     <row r="33" spans="2:7" ht="44" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B33" s="3">
         <v>29</v>
       </c>
-      <c r="C33" s="6" t="s">
-        <v>65</v>
-      </c>
-      <c r="D33" s="6" t="s">
-        <v>62</v>
-      </c>
-      <c r="E33" s="6" t="s">
-        <v>56</v>
-      </c>
-      <c r="F33" s="6" t="s">
-        <v>77</v>
-      </c>
-      <c r="G33" s="6"/>
+      <c r="C33" s="4" t="s">
+        <v>64</v>
+      </c>
+      <c r="D33" s="4" t="s">
+        <v>61</v>
+      </c>
+      <c r="E33" s="4" t="s">
+        <v>55</v>
+      </c>
+      <c r="F33" s="4" t="s">
+        <v>76</v>
+      </c>
+      <c r="G33" s="4"/>
     </row>
     <row r="34" spans="2:7" ht="33.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B34" s="3">
         <v>30</v>
       </c>
-      <c r="C34" s="9" t="s">
-        <v>66</v>
-      </c>
-      <c r="D34" s="10"/>
-      <c r="E34" s="10"/>
-      <c r="F34" s="10"/>
-      <c r="G34" s="11"/>
+      <c r="C34" s="7" t="s">
+        <v>65</v>
+      </c>
+      <c r="D34" s="8"/>
+      <c r="E34" s="8"/>
+      <c r="F34" s="8"/>
+      <c r="G34" s="9"/>
     </row>
     <row r="35" spans="2:7" ht="44" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B35" s="3">
         <v>31</v>
       </c>
-      <c r="C35" s="6" t="s">
+      <c r="C35" s="4" t="s">
+        <v>66</v>
+      </c>
+      <c r="D35" s="4" t="s">
         <v>67</v>
       </c>
-      <c r="D35" s="6" t="s">
-        <v>68</v>
-      </c>
-      <c r="E35" s="6" t="s">
-        <v>96</v>
-      </c>
-      <c r="F35" s="6">
+      <c r="E35" s="4" t="s">
+        <v>95</v>
+      </c>
+      <c r="F35" s="4">
         <v>0</v>
       </c>
-      <c r="G35" s="6"/>
+      <c r="G35" s="4"/>
     </row>
     <row r="36" spans="2:7" ht="32" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B36" s="3">
         <v>32</v>
       </c>
-      <c r="C36" s="9" t="s">
-        <v>71</v>
-      </c>
-      <c r="D36" s="10"/>
-      <c r="E36" s="10"/>
-      <c r="F36" s="10"/>
-      <c r="G36" s="11"/>
+      <c r="C36" s="7" t="s">
+        <v>70</v>
+      </c>
+      <c r="D36" s="8"/>
+      <c r="E36" s="8"/>
+      <c r="F36" s="8"/>
+      <c r="G36" s="9"/>
     </row>
     <row r="37" spans="2:7" ht="44" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B37" s="3">
         <v>33</v>
       </c>
-      <c r="C37" s="6" t="s">
+      <c r="C37" s="4" t="s">
+        <v>68</v>
+      </c>
+      <c r="D37" s="4" t="s">
         <v>69</v>
       </c>
-      <c r="D37" s="6" t="s">
-        <v>70</v>
-      </c>
-      <c r="E37" s="6" t="s">
-        <v>96</v>
-      </c>
-      <c r="F37" s="6" t="s">
-        <v>77</v>
-      </c>
-      <c r="G37" s="6"/>
+      <c r="E37" s="4" t="s">
+        <v>95</v>
+      </c>
+      <c r="F37" s="4" t="s">
+        <v>76</v>
+      </c>
+      <c r="G37" s="4"/>
     </row>
     <row r="38" spans="2:7" ht="32" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B38" s="3">
         <v>34</v>
       </c>
-      <c r="C38" s="9" t="s">
-        <v>72</v>
-      </c>
-      <c r="D38" s="10"/>
-      <c r="E38" s="10"/>
-      <c r="F38" s="10"/>
-      <c r="G38" s="11"/>
+      <c r="C38" s="7" t="s">
+        <v>71</v>
+      </c>
+      <c r="D38" s="8"/>
+      <c r="E38" s="8"/>
+      <c r="F38" s="8"/>
+      <c r="G38" s="9"/>
     </row>
     <row r="39" spans="2:7" ht="44" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B39" s="3">
         <v>35</v>
       </c>
-      <c r="C39" s="6" t="s">
-        <v>73</v>
-      </c>
-      <c r="D39" s="6" t="s">
-        <v>70</v>
-      </c>
-      <c r="E39" s="6" t="s">
-        <v>76</v>
-      </c>
-      <c r="F39" s="6">
+      <c r="C39" s="4" t="s">
+        <v>72</v>
+      </c>
+      <c r="D39" s="4" t="s">
+        <v>69</v>
+      </c>
+      <c r="E39" s="4" t="s">
+        <v>75</v>
+      </c>
+      <c r="F39" s="4">
         <v>0</v>
       </c>
-      <c r="G39" s="6"/>
+      <c r="G39" s="4"/>
     </row>
     <row r="40" spans="2:7" ht="31.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B40" s="3">
         <v>36</v>
       </c>
-      <c r="C40" s="9" t="s">
-        <v>74</v>
-      </c>
-      <c r="D40" s="10"/>
-      <c r="E40" s="10"/>
-      <c r="F40" s="10"/>
-      <c r="G40" s="11"/>
+      <c r="C40" s="7" t="s">
+        <v>73</v>
+      </c>
+      <c r="D40" s="8"/>
+      <c r="E40" s="8"/>
+      <c r="F40" s="8"/>
+      <c r="G40" s="9"/>
     </row>
     <row r="41" spans="2:7" ht="44" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B41" s="3">
         <v>37</v>
       </c>
-      <c r="C41" s="6" t="s">
+      <c r="C41" s="4" t="s">
+        <v>74</v>
+      </c>
+      <c r="D41" s="5" t="s">
+        <v>67</v>
+      </c>
+      <c r="E41" s="5" t="s">
         <v>75</v>
       </c>
-      <c r="D41" s="7" t="s">
-        <v>68</v>
-      </c>
-      <c r="E41" s="7" t="s">
+      <c r="F41" s="5" t="s">
         <v>76</v>
       </c>
-      <c r="F41" s="7" t="s">
-        <v>77</v>
-      </c>
-      <c r="G41" s="7"/>
+      <c r="G41" s="5"/>
     </row>
     <row r="42" spans="2:7" ht="40.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B42" s="3">
         <v>38</v>
       </c>
-      <c r="C42" s="9" t="s">
-        <v>78</v>
-      </c>
-      <c r="D42" s="10"/>
-      <c r="E42" s="10"/>
-      <c r="F42" s="10"/>
-      <c r="G42" s="11"/>
+      <c r="C42" s="7" t="s">
+        <v>77</v>
+      </c>
+      <c r="D42" s="8"/>
+      <c r="E42" s="8"/>
+      <c r="F42" s="8"/>
+      <c r="G42" s="9"/>
     </row>
     <row r="43" spans="2:7" ht="44" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B43" s="3">
         <v>39</v>
       </c>
-      <c r="C43" s="6" t="s">
+      <c r="C43" s="4" t="s">
+        <v>80</v>
+      </c>
+      <c r="D43" s="4" t="s">
+        <v>78</v>
+      </c>
+      <c r="E43" s="4" t="s">
         <v>81</v>
       </c>
-      <c r="D43" s="6" t="s">
+      <c r="F43" s="4" t="s">
         <v>79</v>
       </c>
-      <c r="E43" s="6" t="s">
-        <v>82</v>
-      </c>
-      <c r="F43" s="6" t="s">
-        <v>80</v>
-      </c>
-      <c r="G43" s="6"/>
+      <c r="G43" s="4"/>
     </row>
     <row r="44" spans="2:7" ht="29.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B44" s="3">
         <v>40</v>
       </c>
-      <c r="C44" s="9" t="s">
-        <v>83</v>
-      </c>
-      <c r="D44" s="10"/>
-      <c r="E44" s="10"/>
-      <c r="F44" s="10"/>
-      <c r="G44" s="11"/>
+      <c r="C44" s="7" t="s">
+        <v>82</v>
+      </c>
+      <c r="D44" s="8"/>
+      <c r="E44" s="8"/>
+      <c r="F44" s="8"/>
+      <c r="G44" s="9"/>
     </row>
     <row r="45" spans="2:7" ht="29.5" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B45" s="3">
         <v>41</v>
       </c>
-      <c r="C45" s="6" t="s">
+      <c r="C45" s="4" t="s">
+        <v>83</v>
+      </c>
+      <c r="D45" s="4" t="s">
         <v>84</v>
       </c>
-      <c r="D45" s="6" t="s">
+      <c r="E45" s="4" t="s">
         <v>85</v>
       </c>
-      <c r="E45" s="6" t="s">
-        <v>86</v>
-      </c>
-      <c r="F45" s="6" t="s">
-        <v>88</v>
-      </c>
-      <c r="G45" s="6"/>
+      <c r="F45" s="4" t="s">
+        <v>87</v>
+      </c>
+      <c r="G45" s="4"/>
     </row>
     <row r="46" spans="2:7" ht="34.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B46" s="3">
         <v>42</v>
       </c>
-      <c r="C46" s="9" t="s">
-        <v>87</v>
-      </c>
-      <c r="D46" s="10"/>
-      <c r="E46" s="10"/>
-      <c r="F46" s="10"/>
-      <c r="G46" s="11"/>
+      <c r="C46" s="7" t="s">
+        <v>86</v>
+      </c>
+      <c r="D46" s="8"/>
+      <c r="E46" s="8"/>
+      <c r="F46" s="8"/>
+      <c r="G46" s="9"/>
     </row>
     <row r="47" spans="2:7" ht="58.5" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B47" s="3">
         <v>43</v>
       </c>
-      <c r="C47" s="6" t="s">
+      <c r="C47" s="4" t="s">
+        <v>88</v>
+      </c>
+      <c r="D47" s="4"/>
+      <c r="E47" s="4" t="s">
         <v>89</v>
       </c>
-      <c r="D47" s="6"/>
-      <c r="E47" s="6" t="s">
+      <c r="F47" s="4" t="s">
         <v>90</v>
       </c>
-      <c r="F47" s="6" t="s">
-        <v>91</v>
-      </c>
-      <c r="G47" s="6"/>
+      <c r="G47" s="4"/>
     </row>
     <row r="48" spans="2:7" ht="35.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B48" s="3">
         <v>44</v>
       </c>
-      <c r="C48" s="9" t="s">
-        <v>92</v>
-      </c>
-      <c r="D48" s="10"/>
-      <c r="E48" s="10"/>
-      <c r="F48" s="10"/>
-      <c r="G48" s="11"/>
+      <c r="C48" s="7" t="s">
+        <v>91</v>
+      </c>
+      <c r="D48" s="8"/>
+      <c r="E48" s="8"/>
+      <c r="F48" s="8"/>
+      <c r="G48" s="9"/>
     </row>
     <row r="49" spans="2:7" ht="44" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B49" s="3">
         <v>45</v>
       </c>
-      <c r="C49" s="6" t="s">
-        <v>93</v>
-      </c>
-      <c r="D49" s="6" t="s">
-        <v>68</v>
-      </c>
-      <c r="E49" s="6" t="s">
-        <v>95</v>
-      </c>
-      <c r="F49" s="6">
+      <c r="C49" s="4" t="s">
+        <v>92</v>
+      </c>
+      <c r="D49" s="4" t="s">
+        <v>67</v>
+      </c>
+      <c r="E49" s="4" t="s">
+        <v>94</v>
+      </c>
+      <c r="F49" s="4">
         <v>0</v>
       </c>
-      <c r="G49" s="6"/>
+      <c r="G49" s="4"/>
     </row>
     <row r="50" spans="2:7" ht="34.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B50" s="3">
         <v>46</v>
       </c>
-      <c r="C50" s="9" t="s">
-        <v>94</v>
-      </c>
-      <c r="D50" s="10"/>
-      <c r="E50" s="10"/>
-      <c r="F50" s="10"/>
-      <c r="G50" s="11"/>
+      <c r="C50" s="7" t="s">
+        <v>93</v>
+      </c>
+      <c r="D50" s="8"/>
+      <c r="E50" s="8"/>
+      <c r="F50" s="8"/>
+      <c r="G50" s="9"/>
     </row>
     <row r="51" spans="2:7" ht="44" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B51" s="3">
         <v>47</v>
       </c>
-      <c r="C51" s="6" t="s">
+      <c r="C51" s="4" t="s">
+        <v>96</v>
+      </c>
+      <c r="D51" s="4" t="s">
+        <v>69</v>
+      </c>
+      <c r="E51" s="4" t="s">
+        <v>94</v>
+      </c>
+      <c r="F51" s="4" t="s">
         <v>97</v>
       </c>
-      <c r="D51" s="6" t="s">
-        <v>70</v>
-      </c>
-      <c r="E51" s="6" t="s">
-        <v>95</v>
-      </c>
-      <c r="F51" s="6" t="s">
-        <v>98</v>
-      </c>
-      <c r="G51" s="6"/>
+      <c r="G51" s="4"/>
     </row>
     <row r="52" spans="2:7" ht="34.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B52" s="3">
         <v>48</v>
       </c>
-      <c r="C52" s="9" t="s">
-        <v>99</v>
-      </c>
-      <c r="D52" s="10"/>
-      <c r="E52" s="10"/>
-      <c r="F52" s="10"/>
-      <c r="G52" s="11"/>
+      <c r="C52" s="7" t="s">
+        <v>98</v>
+      </c>
+      <c r="D52" s="8"/>
+      <c r="E52" s="8"/>
+      <c r="F52" s="8"/>
+      <c r="G52" s="9"/>
     </row>
     <row r="53" spans="2:7" ht="58.5" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B53" s="3">
         <v>49</v>
       </c>
-      <c r="C53" s="6" t="s">
+      <c r="C53" s="4" t="s">
+        <v>99</v>
+      </c>
+      <c r="D53" s="4" t="s">
         <v>100</v>
       </c>
-      <c r="D53" s="6" t="s">
+      <c r="E53" s="4" t="s">
         <v>101</v>
       </c>
-      <c r="E53" s="6" t="s">
+      <c r="F53" s="4" t="s">
         <v>102</v>
       </c>
-      <c r="F53" s="6" t="s">
-        <v>103</v>
-      </c>
-      <c r="G53" s="6"/>
+      <c r="G53" s="4"/>
     </row>
     <row r="54" spans="2:7" ht="33" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B54" s="3">
         <v>50</v>
       </c>
-      <c r="C54" s="9" t="s">
-        <v>104</v>
-      </c>
-      <c r="D54" s="10"/>
-      <c r="E54" s="10"/>
-      <c r="F54" s="10"/>
-      <c r="G54" s="11"/>
+      <c r="C54" s="7" t="s">
+        <v>103</v>
+      </c>
+      <c r="D54" s="8"/>
+      <c r="E54" s="8"/>
+      <c r="F54" s="8"/>
+      <c r="G54" s="9"/>
     </row>
     <row r="55" spans="2:7" ht="44" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B55" s="3">
         <v>51</v>
       </c>
-      <c r="C55" s="6" t="s">
+      <c r="C55" s="4" t="s">
+        <v>104</v>
+      </c>
+      <c r="D55" s="4" t="s">
+        <v>100</v>
+      </c>
+      <c r="E55" s="4" t="s">
         <v>105</v>
       </c>
-      <c r="D55" s="6" t="s">
-        <v>101</v>
-      </c>
-      <c r="E55" s="6" t="s">
-        <v>106</v>
-      </c>
-      <c r="F55" s="6" t="s">
-        <v>98</v>
-      </c>
-      <c r="G55" s="6"/>
+      <c r="F55" s="4" t="s">
+        <v>97</v>
+      </c>
+      <c r="G55" s="4"/>
     </row>
     <row r="56" spans="2:7" ht="29.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B56" s="3">
         <v>52</v>
       </c>
-      <c r="C56" s="9" t="s">
-        <v>107</v>
-      </c>
-      <c r="D56" s="10"/>
-      <c r="E56" s="10"/>
-      <c r="F56" s="10"/>
-      <c r="G56" s="11"/>
+      <c r="C56" s="7" t="s">
+        <v>106</v>
+      </c>
+      <c r="D56" s="8"/>
+      <c r="E56" s="8"/>
+      <c r="F56" s="8"/>
+      <c r="G56" s="9"/>
     </row>
     <row r="57" spans="2:7" ht="58.5" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B57" s="3">
         <v>53</v>
       </c>
-      <c r="C57" s="6" t="s">
+      <c r="C57" s="4" t="s">
+        <v>107</v>
+      </c>
+      <c r="D57" s="4"/>
+      <c r="E57" s="4" t="s">
         <v>108</v>
       </c>
-      <c r="D57" s="6"/>
-      <c r="E57" s="6" t="s">
-        <v>109</v>
-      </c>
-      <c r="F57" s="6" t="s">
-        <v>80</v>
-      </c>
-      <c r="G57" s="6"/>
+      <c r="F57" s="4" t="s">
+        <v>79</v>
+      </c>
+      <c r="G57" s="4"/>
     </row>
     <row r="58" spans="2:7" ht="58.5" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B58" s="3">
         <v>54</v>
       </c>
-      <c r="C58" s="6" t="s">
+      <c r="C58" s="4" t="s">
+        <v>109</v>
+      </c>
+      <c r="D58" s="4"/>
+      <c r="E58" s="4" t="s">
         <v>110</v>
       </c>
-      <c r="D58" s="6"/>
-      <c r="E58" s="6" t="s">
-        <v>111</v>
-      </c>
-      <c r="F58" s="6" t="s">
-        <v>80</v>
-      </c>
-      <c r="G58" s="6"/>
+      <c r="F58" s="4" t="s">
+        <v>79</v>
+      </c>
+      <c r="G58" s="4"/>
     </row>
     <row r="59" spans="2:7" ht="31" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B59" s="3">
         <v>55</v>
       </c>
-      <c r="C59" s="9" t="s">
-        <v>112</v>
-      </c>
-      <c r="D59" s="10"/>
-      <c r="E59" s="10"/>
-      <c r="F59" s="10"/>
-      <c r="G59" s="11"/>
+      <c r="C59" s="7" t="s">
+        <v>111</v>
+      </c>
+      <c r="D59" s="8"/>
+      <c r="E59" s="8"/>
+      <c r="F59" s="8"/>
+      <c r="G59" s="9"/>
     </row>
     <row r="60" spans="2:7" ht="29.5" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B60" s="3">
         <v>56</v>
       </c>
-      <c r="C60" s="6" t="s">
-        <v>116</v>
-      </c>
-      <c r="D60" s="6" t="s">
-        <v>113</v>
-      </c>
-      <c r="E60" s="6" t="s">
+      <c r="C60" s="4" t="s">
         <v>115</v>
       </c>
-      <c r="F60" s="6" t="s">
-        <v>80</v>
-      </c>
-      <c r="G60" s="6"/>
+      <c r="D60" s="4" t="s">
+        <v>112</v>
+      </c>
+      <c r="E60" s="4" t="s">
+        <v>114</v>
+      </c>
+      <c r="F60" s="4" t="s">
+        <v>79</v>
+      </c>
+      <c r="G60" s="4"/>
     </row>
     <row r="61" spans="2:7" ht="87.5" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B61" s="3">
         <v>57</v>
       </c>
-      <c r="C61" s="6" t="s">
+      <c r="C61" s="4" t="s">
+        <v>116</v>
+      </c>
+      <c r="D61" s="4"/>
+      <c r="E61" s="4" t="s">
         <v>117</v>
       </c>
-      <c r="D61" s="6"/>
-      <c r="E61" s="6" t="s">
-        <v>118</v>
-      </c>
-      <c r="F61" s="6" t="s">
-        <v>80</v>
-      </c>
-      <c r="G61" s="6"/>
+      <c r="F61" s="4" t="s">
+        <v>79</v>
+      </c>
+      <c r="G61" s="4"/>
     </row>
     <row r="62" spans="2:7" ht="33" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B62" s="3">
         <v>58</v>
       </c>
-      <c r="C62" s="9" t="s">
-        <v>119</v>
-      </c>
-      <c r="D62" s="10"/>
-      <c r="E62" s="10"/>
-      <c r="F62" s="10"/>
-      <c r="G62" s="11"/>
+      <c r="C62" s="7" t="s">
+        <v>118</v>
+      </c>
+      <c r="D62" s="8"/>
+      <c r="E62" s="8"/>
+      <c r="F62" s="8"/>
+      <c r="G62" s="9"/>
     </row>
     <row r="63" spans="2:7" ht="29.5" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B63" s="3">
         <v>59</v>
       </c>
-      <c r="C63" s="6" t="s">
-        <v>114</v>
-      </c>
-      <c r="D63" s="6" t="s">
+      <c r="C63" s="4" t="s">
+        <v>113</v>
+      </c>
+      <c r="D63" s="4" t="s">
+        <v>119</v>
+      </c>
+      <c r="E63" s="4" t="s">
         <v>120</v>
       </c>
-      <c r="E63" s="6" t="s">
-        <v>121</v>
-      </c>
-      <c r="F63" s="6" t="s">
-        <v>80</v>
-      </c>
-      <c r="G63" s="6"/>
+      <c r="F63" s="4" t="s">
+        <v>79</v>
+      </c>
+      <c r="G63" s="4"/>
     </row>
     <row r="64" spans="2:7" ht="44" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B64" s="3">
         <v>60</v>
       </c>
-      <c r="C64" s="6" t="s">
+      <c r="C64" s="4" t="s">
+        <v>121</v>
+      </c>
+      <c r="D64" s="4"/>
+      <c r="E64" s="4" t="s">
         <v>122</v>
       </c>
-      <c r="D64" s="6"/>
-      <c r="E64" s="6" t="s">
-        <v>123</v>
-      </c>
-      <c r="F64" s="6" t="s">
-        <v>80</v>
-      </c>
-      <c r="G64" s="6"/>
-    </row>
-    <row r="65" spans="1:7" ht="35" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="F64" s="4" t="s">
+        <v>79</v>
+      </c>
+      <c r="G64" s="4"/>
+    </row>
+    <row r="65" spans="2:7" ht="35" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B65" s="3">
         <v>61</v>
       </c>
-      <c r="C65" s="9" t="s">
-        <v>124</v>
-      </c>
-      <c r="D65" s="10"/>
-      <c r="E65" s="10"/>
-      <c r="F65" s="10"/>
-      <c r="G65" s="11"/>
-    </row>
-    <row r="66" spans="1:7" ht="73" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="C65" s="7" t="s">
+        <v>123</v>
+      </c>
+      <c r="D65" s="8"/>
+      <c r="E65" s="8"/>
+      <c r="F65" s="8"/>
+      <c r="G65" s="9"/>
+    </row>
+    <row r="66" spans="2:7" ht="73" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B66" s="3">
         <v>62</v>
       </c>
-      <c r="C66" s="6" t="s">
+      <c r="C66" s="4" t="s">
+        <v>124</v>
+      </c>
+      <c r="D66" s="4"/>
+      <c r="E66" s="4" t="s">
         <v>125</v>
       </c>
-      <c r="D66" s="6"/>
-      <c r="E66" s="6" t="s">
-        <v>126</v>
-      </c>
-      <c r="F66" s="6" t="s">
-        <v>80</v>
-      </c>
-      <c r="G66" s="6"/>
-    </row>
-    <row r="67" spans="1:7" ht="23.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A67" t="s">
-        <v>55</v>
-      </c>
+      <c r="F66" s="4" t="s">
+        <v>79</v>
+      </c>
+      <c r="G66" s="4"/>
+    </row>
+    <row r="67" spans="2:7" ht="23.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B67" s="3">
         <v>63</v>
       </c>
-      <c r="C67" s="9" t="s">
-        <v>127</v>
-      </c>
-      <c r="D67" s="10"/>
-      <c r="E67" s="10"/>
-      <c r="F67" s="10"/>
-      <c r="G67" s="11"/>
-    </row>
-    <row r="68" spans="1:7" ht="73" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="C67" s="7" t="s">
+        <v>126</v>
+      </c>
+      <c r="D67" s="8"/>
+      <c r="E67" s="8"/>
+      <c r="F67" s="8"/>
+      <c r="G67" s="9"/>
+    </row>
+    <row r="68" spans="2:7" ht="73" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B68" s="3">
         <v>64</v>
       </c>
-      <c r="C68" s="6" t="s">
+      <c r="C68" s="4" t="s">
+        <v>124</v>
+      </c>
+      <c r="D68" s="4"/>
+      <c r="E68" s="4" t="s">
         <v>125</v>
       </c>
-      <c r="D68" s="6"/>
-      <c r="E68" s="6" t="s">
-        <v>126</v>
-      </c>
-      <c r="F68" s="6" t="s">
-        <v>80</v>
-      </c>
-      <c r="G68" s="6"/>
-    </row>
-    <row r="69" spans="1:7" ht="33" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="F68" s="4" t="s">
+        <v>79</v>
+      </c>
+      <c r="G68" s="4"/>
+    </row>
+    <row r="69" spans="2:7" ht="33" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B69" s="3">
         <v>65</v>
       </c>
-      <c r="C69" s="9" t="s">
-        <v>128</v>
-      </c>
-      <c r="D69" s="10"/>
-      <c r="E69" s="10"/>
-      <c r="F69" s="10"/>
-      <c r="G69" s="11"/>
-    </row>
-    <row r="70" spans="1:7" ht="58.5" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="C69" s="7" t="s">
+        <v>127</v>
+      </c>
+      <c r="D69" s="8"/>
+      <c r="E69" s="8"/>
+      <c r="F69" s="8"/>
+      <c r="G69" s="9"/>
+    </row>
+    <row r="70" spans="2:7" ht="58.5" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B70" s="3">
         <v>66</v>
       </c>
-      <c r="C70" s="6" t="s">
+      <c r="C70" s="4" t="s">
+        <v>129</v>
+      </c>
+      <c r="D70" s="4" t="s">
+        <v>128</v>
+      </c>
+      <c r="E70" s="4" t="s">
         <v>130</v>
       </c>
-      <c r="D70" s="6" t="s">
-        <v>129</v>
-      </c>
-      <c r="E70" s="6" t="s">
-        <v>131</v>
-      </c>
-      <c r="F70" s="6" t="s">
-        <v>80</v>
-      </c>
-      <c r="G70" s="6"/>
-    </row>
-    <row r="71" spans="1:7" ht="23.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="F70" s="4" t="s">
+        <v>79</v>
+      </c>
+      <c r="G70" s="4"/>
+    </row>
+    <row r="71" spans="2:7" ht="23.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B71" s="3">
         <v>67</v>
       </c>
-      <c r="C71" s="9" t="s">
-        <v>132</v>
-      </c>
-      <c r="D71" s="10"/>
-      <c r="E71" s="10"/>
-      <c r="F71" s="10"/>
-      <c r="G71" s="11"/>
-    </row>
-    <row r="72" spans="1:7" ht="58.5" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="C71" s="7" t="s">
+        <v>131</v>
+      </c>
+      <c r="D71" s="8"/>
+      <c r="E71" s="8"/>
+      <c r="F71" s="8"/>
+      <c r="G71" s="9"/>
+    </row>
+    <row r="72" spans="2:7" ht="58.5" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B72" s="3">
         <v>68</v>
       </c>
-      <c r="C72" s="6" t="s">
-        <v>137</v>
-      </c>
-      <c r="D72" s="6" t="s">
-        <v>134</v>
-      </c>
-      <c r="E72" s="6" t="s">
+      <c r="C72" s="4" t="s">
         <v>136</v>
       </c>
-      <c r="F72" s="6">
+      <c r="D72" s="4" t="s">
+        <v>133</v>
+      </c>
+      <c r="E72" s="4" t="s">
+        <v>135</v>
+      </c>
+      <c r="F72" s="4">
         <v>2</v>
       </c>
-      <c r="G72" s="6"/>
-    </row>
-    <row r="73" spans="1:7" ht="23.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="G72" s="4"/>
+    </row>
+    <row r="73" spans="2:7" ht="23.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B73" s="3">
         <v>69</v>
       </c>
-      <c r="C73" s="9" t="s">
-        <v>133</v>
-      </c>
-      <c r="D73" s="10"/>
-      <c r="E73" s="10"/>
-      <c r="F73" s="10"/>
-      <c r="G73" s="11"/>
-    </row>
-    <row r="74" spans="1:7" ht="58.5" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="C73" s="7" t="s">
+        <v>132</v>
+      </c>
+      <c r="D73" s="8"/>
+      <c r="E73" s="8"/>
+      <c r="F73" s="8"/>
+      <c r="G73" s="9"/>
+    </row>
+    <row r="74" spans="2:7" ht="58.5" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B74" s="3">
         <v>70</v>
       </c>
-      <c r="C74" s="6" t="s">
-        <v>138</v>
-      </c>
-      <c r="D74" s="6" t="s">
-        <v>129</v>
-      </c>
-      <c r="E74" s="6" t="s">
-        <v>135</v>
-      </c>
-      <c r="F74" s="6" t="s">
-        <v>80</v>
-      </c>
-      <c r="G74" s="6"/>
+      <c r="C74" s="4" t="s">
+        <v>137</v>
+      </c>
+      <c r="D74" s="4" t="s">
+        <v>128</v>
+      </c>
+      <c r="E74" s="4" t="s">
+        <v>134</v>
+      </c>
+      <c r="F74" s="4" t="s">
+        <v>79</v>
+      </c>
+      <c r="G74" s="4"/>
     </row>
   </sheetData>
   <mergeCells count="32">
+    <mergeCell ref="F2:G2"/>
+    <mergeCell ref="C5:G5"/>
+    <mergeCell ref="C7:G7"/>
+    <mergeCell ref="C9:G9"/>
+    <mergeCell ref="C12:G12"/>
+    <mergeCell ref="C15:G15"/>
+    <mergeCell ref="C17:G17"/>
+    <mergeCell ref="C19:G19"/>
+    <mergeCell ref="C23:G23"/>
+    <mergeCell ref="C25:G25"/>
+    <mergeCell ref="C27:G27"/>
+    <mergeCell ref="C30:G30"/>
+    <mergeCell ref="C32:G32"/>
+    <mergeCell ref="C34:G34"/>
+    <mergeCell ref="C36:G36"/>
+    <mergeCell ref="C38:G38"/>
+    <mergeCell ref="C40:G40"/>
+    <mergeCell ref="C42:G42"/>
+    <mergeCell ref="C44:G44"/>
+    <mergeCell ref="C46:G46"/>
+    <mergeCell ref="C48:G48"/>
+    <mergeCell ref="C50:G50"/>
+    <mergeCell ref="C52:G52"/>
+    <mergeCell ref="C54:G54"/>
+    <mergeCell ref="C56:G56"/>
     <mergeCell ref="C71:G71"/>
     <mergeCell ref="C73:G73"/>
     <mergeCell ref="C59:G59"/>
@@ -2185,31 +2204,6 @@
     <mergeCell ref="C65:G65"/>
     <mergeCell ref="C67:G67"/>
     <mergeCell ref="C69:G69"/>
-    <mergeCell ref="C48:G48"/>
-    <mergeCell ref="C50:G50"/>
-    <mergeCell ref="C52:G52"/>
-    <mergeCell ref="C54:G54"/>
-    <mergeCell ref="C56:G56"/>
-    <mergeCell ref="C38:G38"/>
-    <mergeCell ref="C40:G40"/>
-    <mergeCell ref="C42:G42"/>
-    <mergeCell ref="C44:G44"/>
-    <mergeCell ref="C46:G46"/>
-    <mergeCell ref="C27:G27"/>
-    <mergeCell ref="C30:G30"/>
-    <mergeCell ref="C32:G32"/>
-    <mergeCell ref="C34:G34"/>
-    <mergeCell ref="C36:G36"/>
-    <mergeCell ref="C15:G15"/>
-    <mergeCell ref="C17:G17"/>
-    <mergeCell ref="C19:G19"/>
-    <mergeCell ref="C23:G23"/>
-    <mergeCell ref="C25:G25"/>
-    <mergeCell ref="F2:G2"/>
-    <mergeCell ref="C5:G5"/>
-    <mergeCell ref="C7:G7"/>
-    <mergeCell ref="C9:G9"/>
-    <mergeCell ref="C12:G12"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>